<commit_message>
Notas po si acaso
</commit_message>
<xml_diff>
--- a/Tarea#4.xlsx
+++ b/Tarea#4.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edgar\OneDrive\Documentos\Universidad\13 Treceavo Periodo\Analisis de Algoritmos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edgar\OneDrive\Documentos\Universidad\13 Treceavo Periodo\Analisis de Algoritmos\Tarea-4_AnalisisAlgoritmos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC36940-63B4-4921-A7E7-3147A3D2F7EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594E6F34-9D52-40A8-BB1A-50B36BAFA655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{4FE180B7-E671-4F04-ADC5-C8291E7F4ECC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="32">
   <si>
     <t>BubbleSort</t>
   </si>
@@ -104,15 +104,6 @@
     <t>Mejor:</t>
   </si>
   <si>
-    <t>Suma</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Recuento</t>
-  </si>
-  <si>
     <t>SORTS</t>
   </si>
   <si>
@@ -124,15 +115,33 @@
   <si>
     <t>https://github.com/ColdCrawd/Tarea-4_AnalisisAlgoritmos</t>
   </si>
+  <si>
+    <t xml:space="preserve">Se puede observar que los algoritmos O(n * log n ) en donde el log es de base 2, son los mas rapidos, y tienen un tiempo mas o menos similar. Pero en los algoritmos probados se observa que el QuickSort tiene el mejor </t>
+  </si>
+  <si>
+    <t>Se uso de referencia</t>
+  </si>
+  <si>
+    <t>Copiado</t>
+  </si>
+  <si>
+    <t>Lo hecho</t>
+  </si>
+  <si>
+    <t>de los tiempos, en las tres versiones, con tamaño pequeño, mediano y grande. A pesar de que el bubbleSort es el mas usado, de los probados, es el menos eficiente, y entre mas datos hay, la diferencia es notable.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ademas, se puede observar que la diferencia entre los 3 ultimos sorts no es de tanta, solo el quicksort sobresale. Estan ordenados de peor a mejor, pasa de peor 578s a 0.06s, </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,6 +158,13 @@
     </font>
     <font>
       <sz val="18"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -347,26 +363,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -376,22 +399,58 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
+  <dxfs count="32">
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -404,7 +463,8 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -412,137 +472,123 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.000000"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.000000"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.000000"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.000000"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.000000"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -555,7 +601,8 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -563,140 +610,15 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.000000"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.000000"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.000000"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.000000"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.000000"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
+      <numFmt numFmtId="164" formatCode="0.000000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -712,6 +634,97 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -724,7 +737,8 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -735,13 +749,12 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="0.000000"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <numFmt numFmtId="164" formatCode="0.000000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -754,13 +767,12 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="0.000000"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <numFmt numFmtId="164" formatCode="0.000000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -773,13 +785,12 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="0.000000"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <numFmt numFmtId="164" formatCode="0.000000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -792,13 +803,12 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="0.000000"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <numFmt numFmtId="164" formatCode="0.000000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -811,13 +821,12 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="0.000000"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <numFmt numFmtId="164" formatCode="0.000000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -830,12 +839,11 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -848,8 +856,46 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -5140,16 +5186,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{454D05F8-8EC1-41CB-966A-3FADF1C9E982}" name="Tabla2" displayName="Tabla2" ref="A3:G9" totalsRowShown="0" headerRowDxfId="20" tableBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{454D05F8-8EC1-41CB-966A-3FADF1C9E982}" name="Tabla2" displayName="Tabla2" ref="A3:G9" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="31">
   <autoFilter ref="A3:G9" xr:uid="{454D05F8-8EC1-41CB-966A-3FADF1C9E982}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{D8AF0926-E189-4B00-AF84-1D5AA559A7C5}" name="SORTS" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{E32A5C1D-0E8C-4860-9C39-1CEB1270D7E5}" name="Prueba1" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{6162F4B2-94AE-4610-8433-D4B5A4FA3705}" name="Prueba2" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{1C243411-F523-4B98-AD28-479B34BFA33A}" name="Prueba3" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{411E5024-E15F-4BB0-9784-E32786F02D9E}" name="Prueba4" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{D2B289A3-25F9-42D9-8650-63D4D20DEF74}" name="Prueba5" dataDxfId="22"/>
-    <tableColumn id="7" xr3:uid="{8073BD76-0291-4261-9C25-19E4BA114F13}" name="Promedio" dataDxfId="21">
+    <tableColumn id="1" xr3:uid="{D8AF0926-E189-4B00-AF84-1D5AA559A7C5}" name="SORTS" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{E32A5C1D-0E8C-4860-9C39-1CEB1270D7E5}" name="Prueba1" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{6162F4B2-94AE-4610-8433-D4B5A4FA3705}" name="Prueba2" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{1C243411-F523-4B98-AD28-479B34BFA33A}" name="Prueba3" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{411E5024-E15F-4BB0-9784-E32786F02D9E}" name="Prueba4" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{D2B289A3-25F9-42D9-8650-63D4D20DEF74}" name="Prueba5" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{8073BD76-0291-4261-9C25-19E4BA114F13}" name="Promedio" dataDxfId="20">
       <calculatedColumnFormula>SUM(B4:F4)/5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5158,16 +5204,16 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{95457C34-0182-4663-84FA-D9CADDCB6876}" name="Tabla3" displayName="Tabla3" ref="I3:O9" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="18" tableBorderDxfId="19" totalsRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{95457C34-0182-4663-84FA-D9CADDCB6876}" name="Tabla3" displayName="Tabla3" ref="I3:O9" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
   <autoFilter ref="I3:O9" xr:uid="{95457C34-0182-4663-84FA-D9CADDCB6876}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{A990C91B-BCD7-4EBC-A5AE-82C245A1BC42}" name="SORTS" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{D8ABA95B-C3EA-41BC-946E-C9E97ACCD847}" name="Prueba1" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{419A8BF1-302E-42E4-9183-B84208056617}" name="Prueba2" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{33C0E949-FFD5-4ABC-9257-F3D814872FE3}" name="Prueba3" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{068C6A0D-3614-4F29-B396-9564589B877C}" name="Prueba4" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{3AE23AB0-B2F0-4156-9B3C-9CA2BB9833C9}" name="Prueba5" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{BBEF9833-CB8F-45E8-897C-697187921EF6}" name="Promedio" dataDxfId="10">
+    <tableColumn id="1" xr3:uid="{A990C91B-BCD7-4EBC-A5AE-82C245A1BC42}" name="SORTS" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{D8ABA95B-C3EA-41BC-946E-C9E97ACCD847}" name="Prueba1" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{419A8BF1-302E-42E4-9183-B84208056617}" name="Prueba2" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{33C0E949-FFD5-4ABC-9257-F3D814872FE3}" name="Prueba3" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{068C6A0D-3614-4F29-B396-9564589B877C}" name="Prueba4" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{3AE23AB0-B2F0-4156-9B3C-9CA2BB9833C9}" name="Prueba5" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{BBEF9833-CB8F-45E8-897C-697187921EF6}" name="Promedio" dataDxfId="11">
       <calculatedColumnFormula>SUM(J4:N4)/5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5176,16 +5222,16 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{07D92F12-3C08-4F0B-89B3-D568969FAEF6}" name="Tabla4" displayName="Tabla4" ref="Q3:W9" totalsRowShown="0" headerRowDxfId="0" tableBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{07D92F12-3C08-4F0B-89B3-D568969FAEF6}" name="Tabla4" displayName="Tabla4" ref="Q3:W9" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" tableBorderDxfId="27">
   <autoFilter ref="Q3:W9" xr:uid="{07D92F12-3C08-4F0B-89B3-D568969FAEF6}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{A5810CEF-D599-4CF7-ACEC-1AB6EE66CCF9}" name="SORTS" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{E5D13852-E64F-4929-A1FC-F6321BE4EA9F}" name="Prueba1" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{19892424-6DFA-4A46-8D56-4498FC7909A2}" name="Prueba2" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{F3C8605B-AC59-405D-B6CA-5C9B7750B7DB}" name="Prueba3" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{AB741867-8518-44C0-A833-E2E81F1C510E}" name="Prueba4" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{CA11D920-4231-4FFD-8874-AF14F0EF4462}" name="Prueba5" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{03E5247B-192F-4766-8B02-4B77CE4E97E3}" name="Promedio" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{A5810CEF-D599-4CF7-ACEC-1AB6EE66CCF9}" name="SORTS" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{E5D13852-E64F-4929-A1FC-F6321BE4EA9F}" name="Prueba1" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{19892424-6DFA-4A46-8D56-4498FC7909A2}" name="Prueba2" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{F3C8605B-AC59-405D-B6CA-5C9B7750B7DB}" name="Prueba3" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{AB741867-8518-44C0-A833-E2E81F1C510E}" name="Prueba4" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{CA11D920-4231-4FFD-8874-AF14F0EF4462}" name="Prueba5" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{03E5247B-192F-4766-8B02-4B77CE4E97E3}" name="Promedio" dataDxfId="2">
       <calculatedColumnFormula>SUM(R4:V4)/5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5510,443 +5556,466 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D40983F-8940-47E0-B47C-49974DCF3035}">
-  <dimension ref="A1:AE31"/>
+  <dimension ref="A1:AF33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="75" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="22" max="22" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:32" ht="24" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="20"/>
-      <c r="I1" s="18" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="9"/>
+      <c r="I1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="20"/>
-      <c r="Q1" s="18" t="s">
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="9"/>
+      <c r="Q1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="20"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="9"/>
     </row>
-    <row r="2" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B2" s="15" t="s">
+    <row r="2" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="17"/>
-      <c r="J2" s="15" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="14"/>
+      <c r="J2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="17"/>
-      <c r="R2" s="15" t="s">
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="14"/>
+      <c r="R2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16"/>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16"/>
-      <c r="W2" s="17"/>
+      <c r="S2" s="13"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="13"/>
+      <c r="W2" s="14"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="12" t="s">
+      <c r="H3" s="15"/>
+      <c r="I3" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="M3" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="N3" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="13" t="s">
+      <c r="O3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="Q3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R3" s="3" t="s">
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="S3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="T3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="U3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="V3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="W3" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="AA3" s="2" t="s">
+      <c r="AA3" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="AB3" s="2"/>
-      <c r="AC3" s="2"/>
-      <c r="AD3" s="2"/>
-      <c r="AE3" s="2"/>
+      <c r="AB3" s="11"/>
+      <c r="AC3" s="11"/>
+      <c r="AD3" s="11"/>
+      <c r="AE3" s="11"/>
+      <c r="AF3" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>3.8630999999999999E-2</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>4.0048E-2</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>3.8995000000000002E-2</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>3.9552999999999998E-2</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>5.3027999999999999E-2</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="20">
         <f>SUM(B4:F4)/5</f>
         <v>4.2050999999999998E-2</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="H4" s="15"/>
+      <c r="I4" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="4">
         <v>22.354465000000001</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="4">
         <v>22.405628</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="4">
         <v>22.48368</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="4">
         <v>22.349807999999999</v>
       </c>
-      <c r="N4" s="5">
+      <c r="N4" s="4">
         <v>22.322731999999998</v>
       </c>
-      <c r="O4" s="6">
+      <c r="O4" s="20">
         <f t="shared" ref="O4:O9" si="0">SUM(J4:N4)/5</f>
         <v>22.383262600000002</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="P4" s="15"/>
+      <c r="Q4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="R4" s="5">
+      <c r="R4" s="4">
         <v>578.64825399999995</v>
       </c>
-      <c r="S4" s="5">
+      <c r="S4" s="4">
         <v>594.35511099999997</v>
       </c>
-      <c r="T4" s="5">
+      <c r="T4" s="4">
         <v>568.97325999999998</v>
       </c>
-      <c r="U4" s="5">
+      <c r="U4" s="4">
         <v>569.739375</v>
       </c>
-      <c r="V4" s="5">
+      <c r="V4" s="4">
         <v>581.32273199999997</v>
       </c>
-      <c r="W4" s="6">
+      <c r="W4" s="20">
         <f t="shared" ref="W4:W9" si="1">SUM(R4:V4)/5</f>
         <v>578.6077464</v>
       </c>
       <c r="Y4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="AA4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="AB4" s="4" t="s">
+      <c r="AB4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="AC4" s="4"/>
-      <c r="AD4" s="4"/>
-      <c r="AE4" s="4"/>
+      <c r="AC4" s="10"/>
+      <c r="AD4" s="10"/>
+      <c r="AE4" s="10"/>
+      <c r="AF4" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>2.5602E-2</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>2.3389E-2</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>2.1957000000000001E-2</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>2.2433999999999999E-2</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>2.2294000000000001E-2</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="20">
         <f>SUM(B5:F5)/5</f>
         <v>2.3135200000000002E-2</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="H5" s="15"/>
+      <c r="I5" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="4">
         <v>8.7384129999999995</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="4">
         <v>8.7403490000000001</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="4">
         <v>8.7378400000000003</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5" s="4">
         <v>8.7695869999999996</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="4">
         <v>8.711487</v>
       </c>
-      <c r="O5" s="6">
+      <c r="O5" s="20">
         <f>SUM(J5:N5)/5</f>
         <v>8.7395352000000006</v>
       </c>
-      <c r="Q5" s="3" t="s">
+      <c r="P5" s="15"/>
+      <c r="Q5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="R5" s="5">
+      <c r="R5" s="4">
         <v>219.31112300000001</v>
       </c>
-      <c r="S5" s="5">
+      <c r="S5" s="4">
         <v>218.86355</v>
       </c>
-      <c r="T5" s="5">
+      <c r="T5" s="4">
         <v>219.58787100000001</v>
       </c>
-      <c r="U5" s="5">
+      <c r="U5" s="4">
         <v>219.78796299999999</v>
       </c>
-      <c r="V5" s="5">
+      <c r="V5" s="4">
         <v>223.507384</v>
       </c>
-      <c r="W5" s="6">
+      <c r="W5" s="20">
         <f>SUM(R5:V5)/5</f>
         <v>220.21157819999999</v>
       </c>
       <c r="AA5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="AB5" s="4" t="s">
+      <c r="AB5" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="AC5" s="4"/>
-      <c r="AD5" s="4"/>
-      <c r="AE5" s="4"/>
+      <c r="AC5" s="10"/>
+      <c r="AD5" s="10"/>
+      <c r="AE5" s="10"/>
+      <c r="AF5" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>1.0253E-2</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>1.1285999999999999E-2</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>1.3209E-2</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>1.0097999999999999E-2</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>9.9030000000000003E-3</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="20">
         <f t="shared" ref="G6:G9" si="2">SUM(B6:F6)/5</f>
         <v>1.0949799999999999E-2</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="H6" s="15"/>
+      <c r="I6" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="4">
         <v>3.7343959999999998</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="4">
         <v>3.7564790000000001</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="4">
         <v>3.7320799999999998</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="4">
         <v>3.730035</v>
       </c>
-      <c r="N6" s="5">
+      <c r="N6" s="4">
         <v>3.7324459999999999</v>
       </c>
-      <c r="O6" s="6">
+      <c r="O6" s="20">
         <f t="shared" si="0"/>
         <v>3.7370871999999999</v>
       </c>
-      <c r="Q6" s="3" t="s">
+      <c r="P6" s="15"/>
+      <c r="Q6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="R6" s="5">
+      <c r="R6" s="4">
         <v>93.666236999999995</v>
       </c>
-      <c r="S6" s="5">
+      <c r="S6" s="4">
         <v>93.873160999999996</v>
       </c>
-      <c r="T6" s="5">
+      <c r="T6" s="4">
         <v>93.442939999999993</v>
       </c>
-      <c r="U6" s="3">
+      <c r="U6" s="2">
         <v>96.622591999999997</v>
       </c>
-      <c r="V6" s="5">
+      <c r="V6" s="4">
         <v>93.644041000000001</v>
       </c>
-      <c r="W6" s="6">
+      <c r="W6" s="20">
         <f t="shared" si="1"/>
         <v>94.249794200000011</v>
       </c>
       <c r="AA6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AB6" s="4" t="s">
+      <c r="AB6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="AC6" s="4"/>
-      <c r="AD6" s="4"/>
-      <c r="AE6" s="4"/>
+      <c r="AC6" s="10"/>
+      <c r="AD6" s="10"/>
+      <c r="AE6" s="10"/>
+      <c r="AF6" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>1.6540000000000001E-3</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>1.243E-3</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>1.25E-3</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>1.4289999999999999E-3</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>1.2620000000000001E-3</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="20">
         <f t="shared" si="2"/>
         <v>1.3676000000000001E-3</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="H7" s="15"/>
+      <c r="I7" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="4">
         <v>2.9680000000000002E-2</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="4">
         <v>2.9481E-2</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="4">
         <v>3.3078999999999997E-2</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="4">
         <v>2.946E-2</v>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" s="4">
         <v>2.928E-2</v>
       </c>
-      <c r="O7" s="6">
+      <c r="O7" s="20">
         <f t="shared" si="0"/>
         <v>3.0196000000000001E-2</v>
       </c>
-      <c r="Q7" s="3" t="s">
+      <c r="P7" s="15"/>
+      <c r="Q7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="R7" s="5">
+      <c r="R7" s="4">
         <v>0.15643799999999999</v>
       </c>
-      <c r="S7" s="5">
+      <c r="S7" s="4">
         <v>0.15707299999999999</v>
       </c>
-      <c r="T7" s="3">
+      <c r="T7" s="2">
         <v>0.15712200000000001</v>
       </c>
-      <c r="U7" s="3">
+      <c r="U7" s="2">
         <v>0.15681700000000001</v>
       </c>
-      <c r="V7" s="5">
+      <c r="V7" s="4">
         <v>0.15617700000000001</v>
       </c>
-      <c r="W7" s="6">
+      <c r="W7" s="20">
         <f t="shared" si="1"/>
         <v>0.15672539999999999</v>
       </c>
@@ -5954,150 +6023,154 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>1.2099999999999999E-3</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>8.4599999999999996E-4</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>7.3499999999999998E-4</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>1.14E-3</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>1.0219999999999999E-3</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="20">
         <f t="shared" si="2"/>
         <v>9.905999999999999E-4</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="H8" s="15"/>
+      <c r="I8" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="4">
         <v>1.9951E-2</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="4">
         <v>2.0187E-2</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="4">
         <v>1.9879000000000001E-2</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="4">
         <v>2.0097E-2</v>
       </c>
-      <c r="N8" s="5">
+      <c r="N8" s="4">
         <v>1.9772000000000001E-2</v>
       </c>
-      <c r="O8" s="6">
+      <c r="O8" s="20">
         <f t="shared" si="0"/>
         <v>1.9977200000000001E-2</v>
       </c>
-      <c r="Q8" s="3" t="s">
+      <c r="P8" s="15"/>
+      <c r="Q8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="R8" s="5">
+      <c r="R8" s="4">
         <v>0.119085</v>
       </c>
-      <c r="S8" s="5">
+      <c r="S8" s="4">
         <v>0.114935</v>
       </c>
-      <c r="T8" s="5">
+      <c r="T8" s="4">
         <v>0.11594699999999999</v>
       </c>
-      <c r="U8" s="5">
+      <c r="U8" s="4">
         <v>0.115605</v>
       </c>
-      <c r="V8" s="5">
+      <c r="V8" s="4">
         <v>0.115617</v>
       </c>
-      <c r="W8" s="6">
+      <c r="W8" s="20">
         <f t="shared" si="1"/>
         <v>0.11623780000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A9" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="26">
         <v>4.15E-4</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="26">
         <v>3.9399999999999998E-4</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="26">
         <v>4.9700000000000005E-4</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="26">
         <v>3.9800000000000002E-4</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="26">
         <v>7.1599999999999995E-4</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="27">
         <f t="shared" si="2"/>
         <v>4.8400000000000006E-4</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="H9" s="15"/>
+      <c r="I9" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="8">
+      <c r="J9" s="26">
         <v>1.0661E-2</v>
       </c>
-      <c r="K9" s="8">
+      <c r="K9" s="26">
         <v>1.1443E-2</v>
       </c>
-      <c r="L9" s="8">
+      <c r="L9" s="26">
         <v>1.0586999999999999E-2</v>
       </c>
-      <c r="M9" s="8">
+      <c r="M9" s="26">
         <v>1.0671E-2</v>
       </c>
-      <c r="N9" s="8">
+      <c r="N9" s="26">
         <v>1.0718E-2</v>
       </c>
-      <c r="O9" s="9">
+      <c r="O9" s="27">
         <f t="shared" si="0"/>
         <v>1.0815999999999999E-2</v>
       </c>
-      <c r="Q9" s="7" t="s">
+      <c r="P9" s="15"/>
+      <c r="Q9" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="R9" s="8">
+      <c r="R9" s="26">
         <v>6.8773000000000001E-2</v>
       </c>
-      <c r="S9" s="8">
+      <c r="S9" s="26">
         <v>6.6543000000000005E-2</v>
       </c>
-      <c r="T9" s="8">
+      <c r="T9" s="26">
         <v>6.4935000000000007E-2</v>
       </c>
-      <c r="U9" s="8">
+      <c r="U9" s="26">
         <v>6.6369999999999998E-2</v>
       </c>
-      <c r="V9" s="8">
+      <c r="V9" s="26">
         <v>6.7585999999999993E-2</v>
       </c>
-      <c r="W9" s="9">
+      <c r="W9" s="27">
         <f t="shared" si="1"/>
         <v>6.6841399999999995E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="5" t="s">
@@ -6120,65 +6193,142 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="30" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="31" spans="2:10" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B31" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="20"/>
+    <row r="29" spans="2:22" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
+      <c r="M29" s="18"/>
+      <c r="N29" s="18"/>
+      <c r="O29" s="18"/>
+      <c r="P29" s="18"/>
+      <c r="Q29" s="18"/>
+      <c r="R29" s="18"/>
+      <c r="S29" s="18"/>
+      <c r="T29" s="18"/>
+      <c r="U29" s="18"/>
+      <c r="V29" s="19"/>
+    </row>
+    <row r="30" spans="2:22" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
+      <c r="M30" s="18"/>
+      <c r="N30" s="18"/>
+      <c r="O30" s="18"/>
+      <c r="P30" s="18"/>
+      <c r="Q30" s="18"/>
+      <c r="R30" s="18"/>
+      <c r="S30" s="18"/>
+      <c r="T30" s="18"/>
+      <c r="U30" s="18"/>
+      <c r="V30" s="19"/>
+    </row>
+    <row r="31" spans="2:22" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16"/>
+      <c r="M31" s="16"/>
+      <c r="N31" s="16"/>
+      <c r="O31" s="16"/>
+      <c r="P31" s="16"/>
+      <c r="Q31" s="16"/>
+      <c r="R31" s="16"/>
+      <c r="S31" s="16"/>
+      <c r="T31" s="16"/>
+      <c r="U31" s="16"/>
+    </row>
+    <row r="32" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="33" spans="2:10" ht="24" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B33" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="C31:J31"/>
-    <mergeCell ref="AB4:AE4"/>
-    <mergeCell ref="AB5:AE5"/>
-    <mergeCell ref="AB6:AE6"/>
-    <mergeCell ref="AA3:AE3"/>
+  <mergeCells count="14">
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="J2:O2"/>
     <mergeCell ref="R2:W2"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="I1:O1"/>
     <mergeCell ref="Q1:W1"/>
+    <mergeCell ref="C33:J33"/>
+    <mergeCell ref="AB4:AE4"/>
+    <mergeCell ref="AB5:AE5"/>
+    <mergeCell ref="AB6:AE6"/>
+    <mergeCell ref="AA3:AE3"/>
+    <mergeCell ref="B30:U30"/>
+    <mergeCell ref="B29:U29"/>
+    <mergeCell ref="B31:U31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>